<commit_message>
Some problem fixed and charts --++
</commit_message>
<xml_diff>
--- a/MedicalProject/file.xlsx
+++ b/MedicalProject/file.xlsx
@@ -41,13 +41,13 @@
     <t>Elmar Qara</t>
   </si>
   <si>
-    <t>Rejected</t>
-  </si>
-  <si>
     <t>Ferid Abdull</t>
   </si>
   <si>
     <t>eqarayev4@std.beu.edu.az</t>
+  </si>
+  <si>
+    <t>Rejected</t>
   </si>
 </sst>
 </file>
@@ -153,15 +153,15 @@
         <v>36</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="0">
         <v>927</v>
@@ -172,16 +172,16 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0">
         <v>231</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PIE chart done for dashboard page
</commit_message>
<xml_diff>
--- a/MedicalProject/file.xlsx
+++ b/MedicalProject/file.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Full Name</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Rejected</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -184,6 +187,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0">
+        <v>1794</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bug and added new features
</commit_message>
<xml_diff>
--- a/MedicalProject/file.xlsx
+++ b/MedicalProject/file.xlsx
@@ -32,22 +32,22 @@
     <t>elmarqarayev69@gmail.com</t>
   </si>
   <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Canceled</t>
+  </si>
+  <si>
+    <t>Elmar Qara</t>
+  </si>
+  <si>
     <t>Accepted</t>
   </si>
   <si>
-    <t>Canceled</t>
-  </si>
-  <si>
-    <t>Elmar Qara</t>
-  </si>
-  <si>
     <t>Ferid Abdull</t>
   </si>
   <si>
     <t>eqarayev4@std.beu.edu.az</t>
-  </si>
-  <si>
-    <t>Rejected</t>
   </si>
   <si>
     <t>Pending</t>
@@ -97,7 +97,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -156,35 +156,35 @@
         <v>36</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0">
         <v>927</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0">
         <v>231</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -198,6 +198,20 @@
         <v>1794</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0">
+        <v>36</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added layer for swargen and layout view bug fixed
</commit_message>
<xml_diff>
--- a/MedicalProject/file.xlsx
+++ b/MedicalProject/file.xlsx
@@ -91,7 +91,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -181,6 +181,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0">
+        <v>312</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Signal R -- doesn't work
</commit_message>
<xml_diff>
--- a/MedicalProject/file.xlsx
+++ b/MedicalProject/file.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Full Name</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Elmar Garayev</t>
+  </si>
+  <si>
+    <t>elmareg@code.edu.az</t>
   </si>
 </sst>
 </file>
@@ -91,7 +97,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -147,7 +153,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="0">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>9</v>
@@ -192,6 +198,48 @@
         <v>312</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0">
+        <v>396</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0">
+        <v>156</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="0">
+        <v>66</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Signal R done For Admin Dashboard
</commit_message>
<xml_diff>
--- a/MedicalProject/file.xlsx
+++ b/MedicalProject/file.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Full Name</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>elmareg@code.edu.az</t>
+  </si>
+  <si>
+    <t>Farid Abdull</t>
+  </si>
+  <si>
+    <t>eqarayev4@std.beu.edu.az</t>
   </si>
 </sst>
 </file>
@@ -97,7 +103,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -198,7 +204,7 @@
         <v>312</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -226,7 +232,7 @@
         <v>156</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -240,7 +246,105 @@
         <v>66</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="0">
+        <v>66</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="0">
+        <v>156</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="0">
+        <v>66</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="0">
+        <v>156</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="0">
+        <v>27</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="0">
+        <v>9</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="0">
+        <v>18</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed verify email for register
</commit_message>
<xml_diff>
--- a/MedicalProject/file.xlsx
+++ b/MedicalProject/file.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Full Name</t>
   </si>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t>elmareg@code.edu.az</t>
-  </si>
-  <si>
-    <t>Farid Abdull</t>
-  </si>
-  <si>
-    <t>eqarayev4@std.beu.edu.az</t>
   </si>
 </sst>
 </file>
@@ -103,7 +97,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -251,13 +245,13 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C11" s="0">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>10</v>
@@ -265,27 +259,27 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C12" s="0">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C13" s="0">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>9</v>
@@ -293,13 +287,13 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C14" s="0">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>9</v>
@@ -316,49 +310,7 @@
         <v>27</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="0">
-        <v>9</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="0">
-        <v>18</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="0">
-        <v>156</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some bug added basketItemsforViewAll
</commit_message>
<xml_diff>
--- a/MedicalProject/file.xlsx
+++ b/MedicalProject/file.xlsx
@@ -97,7 +97,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -313,6 +313,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="0">
+        <v>222</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>